<commit_message>
Transform to MVC model
</commit_message>
<xml_diff>
--- a/public/uploads/stocks/stock_list_22.xlsx
+++ b/public/uploads/stocks/stock_list_22.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -660,7 +660,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="65" zoomScalePageLayoutView="98" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -817,7 +817,9 @@
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
@@ -827,8 +829,12 @@
       <c r="E4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="11"/>
+      <c r="F4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="H4" s="6">
         <v>453543</v>
       </c>
@@ -864,8 +870,12 @@
       <c r="D5" s="16">
         <v>1</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="6"/>
+      <c r="E5" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="G5" s="11" t="s">
         <v>27</v>
       </c>
@@ -881,7 +891,9 @@
       <c r="K5" s="6">
         <v>43</v>
       </c>
-      <c r="L5" s="6"/>
+      <c r="L5" s="6">
+        <v>432</v>
+      </c>
       <c r="M5" s="6">
         <v>4</v>
       </c>
@@ -920,7 +932,9 @@
       <c r="J6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="6"/>
+      <c r="K6" s="6">
+        <v>45</v>
+      </c>
       <c r="L6" s="6">
         <v>35</v>
       </c>
@@ -938,7 +952,9 @@
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D7" s="16">
         <v>1</v>
       </c>
@@ -954,7 +970,9 @@
       <c r="H7" s="6">
         <v>43543543</v>
       </c>
-      <c r="I7" s="19"/>
+      <c r="I7" s="19">
+        <v>42715</v>
+      </c>
       <c r="J7" s="6" t="s">
         <v>34</v>
       </c>
@@ -964,8 +982,12 @@
       <c r="L7" s="6">
         <v>432</v>
       </c>
-      <c r="M7" s="6"/>
-      <c r="N7" s="3"/>
+      <c r="M7" s="6">
+        <v>4</v>
+      </c>
+      <c r="N7" s="3">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">

</xml_diff>